<commit_message>
updating scripts and figures
</commit_message>
<xml_diff>
--- a/CellCounts/DeMMO_Biofilm_CellCounts.xlsx
+++ b/CellCounts/DeMMO_Biofilm_CellCounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Caitlin/Desktop/DeMMO_Pubs/DeMMO_BiofilmPub2019/CellCounts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA39E7EE-E541-B741-B119-DDEDD4EF64AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282ECBDC-93CA-BE45-B39B-C204FF5586DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15920" activeTab="2" xr2:uid="{79752199-1EA7-42AB-AADF-92D0EF32636E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15920" xr2:uid="{79752199-1EA7-42AB-AADF-92D0EF32636E}"/>
   </bookViews>
   <sheets>
     <sheet name="cellCounts" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7555" uniqueCount="1400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7619" uniqueCount="1432">
   <si>
     <t>Site</t>
   </si>
@@ -4233,6 +4233,102 @@
   </si>
   <si>
     <t>filament</t>
+  </si>
+  <si>
+    <t>morphology notes</t>
+  </si>
+  <si>
+    <t>0.2 um rods, 0.2 um filaments, gallionella stalks</t>
+  </si>
+  <si>
+    <t>0.2-0.8um cocci, 0.2um rods, 0.2um filaments, eps</t>
+  </si>
+  <si>
+    <t>0.2um coccobacillus, 0.2-0.5um rods, 0.2-0.5filaments, 0.2-1um cocci, eps, gallionella, 0.4 spirillum</t>
+  </si>
+  <si>
+    <t>0.2 cocci, 0.2um rods, 0.2um filament, eps, gallionella</t>
+  </si>
+  <si>
+    <t>0.2-0.4 rods, 0.2 filaments, 0.4 coccobacillus, 0.2-1um cocci, gallionella, eps</t>
+  </si>
+  <si>
+    <t>0.2-0.4 rods, 0.2um cocci, 0.2 filaments, 0.4 coccobacillus, 0.4 vibrio, gallionella</t>
+  </si>
+  <si>
+    <t>0.2-0.5 rods, 0.2-0. filament, 0.2-0.3 cocci</t>
+  </si>
+  <si>
+    <t>0.2-0.4 rods, 0.2-0.4 filaments, 0.5 coccobacillus, gallionella, eps</t>
+  </si>
+  <si>
+    <t>0.2 rods, 0.2 filaments, 0.3 cocci, 0.2 coccobacillus, eps</t>
+  </si>
+  <si>
+    <t>0.2 rods, 0.2 filaments</t>
+  </si>
+  <si>
+    <t>0.2 rods, 1um cocci, 1um rectangle (very angular with appendages surrounding it)</t>
+  </si>
+  <si>
+    <t>0.2 rods, 0.5 coccobacillus, 0.2 filaments, eps</t>
+  </si>
+  <si>
+    <t>0.2 rods, 0.2 coccobacillus, 0.1 filaments</t>
+  </si>
+  <si>
+    <t>0.2-0.5um rods, 0.2 filaments, 0.2 cocci, 0.2um coccobacillus, gallionella</t>
+  </si>
+  <si>
+    <t>0.2 rods, 0.2 filaments, 0.2 vibrio</t>
+  </si>
+  <si>
+    <t>0.2 rod, 0.2 vibro, 0.2 coccobacillus, gallionella, 0.3 cocci</t>
+  </si>
+  <si>
+    <t>0.2 virio, 0.2 cocci, 0.2 rod</t>
+  </si>
+  <si>
+    <t>0.2-0.5um rods, 0.5um cocci</t>
+  </si>
+  <si>
+    <t>0.2-0.4 rods, 0.2 vibrio, 0.2 spirochetes</t>
+  </si>
+  <si>
+    <t>rods</t>
+  </si>
+  <si>
+    <t>cocci</t>
+  </si>
+  <si>
+    <t>filaments</t>
+  </si>
+  <si>
+    <t>spirochetes</t>
+  </si>
+  <si>
+    <t>gallionella</t>
+  </si>
+  <si>
+    <t>0.2-0.5</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>eps</t>
+  </si>
+  <si>
+    <t>0.2-1</t>
+  </si>
+  <si>
+    <t>0.2-0.4</t>
+  </si>
+  <si>
+    <t>0.2-0.8</t>
+  </si>
+  <si>
+    <t>0.2-0.3</t>
   </si>
 </sst>
 </file>
@@ -4959,11 +5055,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8541FA0D-EE56-4ACF-946F-DD9196494A73}">
-  <dimension ref="A1:M1046"/>
+  <dimension ref="A1:U1046"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="134" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -4979,7 +5075,7 @@
     <col min="10" max="16384" width="9.1640625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="29" customFormat="1">
+    <row r="1" spans="1:21" s="29" customFormat="1">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -5010,8 +5106,41 @@
       <c r="J1" s="29" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="29" t="s">
+        <v>1420</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>1421</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>1393</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>1395</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>1422</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>1397</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>1423</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>1396</v>
+      </c>
+      <c r="S1" s="29" t="s">
+        <v>1424</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>1427</v>
+      </c>
+      <c r="U1" s="29" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="34" t="s">
         <v>137</v>
       </c>
@@ -5045,8 +5174,23 @@
         <f>SUM(DeMMO1!L2:L21)</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="30" t="s">
+        <v>1425</v>
+      </c>
+      <c r="M2" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="O2" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="S2" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="34" t="s">
         <v>137</v>
       </c>
@@ -5081,7 +5225,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:21">
       <c r="A4" s="34" t="s">
         <v>137</v>
       </c>
@@ -5115,8 +5259,26 @@
         <f>SUM(DeMMO1!L47:L68)</f>
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="L4" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="M4" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="P4" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="S4" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U4" s="30" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="34" t="s">
         <v>137</v>
       </c>
@@ -5150,8 +5312,23 @@
         <f>SUM(DeMMO1!L69:L88)</f>
         <v>449</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="M5" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="T5" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U5" s="30" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="34" t="s">
         <v>137</v>
       </c>
@@ -5186,7 +5363,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:21">
       <c r="A7" s="34" t="s">
         <v>137</v>
       </c>
@@ -5220,8 +5397,20 @@
         <f>SUM(DeMMO1!L102:L122)</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="L7" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="M7" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="O7" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="U7" s="30" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="34" t="s">
         <v>137</v>
       </c>
@@ -5255,8 +5444,20 @@
         <f>SUM(DeMMO1!L123:L132)</f>
         <v>1559</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="O8" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="P8" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="U8" s="30" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="34" t="s">
         <v>137</v>
       </c>
@@ -5289,7 +5490,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:21">
       <c r="A10" s="34" t="s">
         <v>137</v>
       </c>
@@ -5323,8 +5524,32 @@
         <f>SUM(DeMMO1!L133:L150)</f>
         <v>4155</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="30" t="s">
+        <v>1425</v>
+      </c>
+      <c r="L10" s="30" t="s">
+        <v>1428</v>
+      </c>
+      <c r="M10" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="O10" s="30" t="s">
+        <v>1425</v>
+      </c>
+      <c r="R10" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="S10" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="T10" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U10" s="30" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="34" t="s">
         <v>137</v>
       </c>
@@ -5358,8 +5583,26 @@
         <f>SUM(DeMMO1!L151:L168)</f>
         <v>1684</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="L11" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="O11" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="S11" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="T11" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U11" s="30" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" s="34" t="s">
         <v>137</v>
       </c>
@@ -5393,8 +5636,26 @@
         <f>SUM(DeMMO1!L169:L179)</f>
         <v>472</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" s="30" t="s">
+        <v>1429</v>
+      </c>
+      <c r="M12" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="O12" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="P12" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="S12" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U12" s="30" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="34" t="s">
         <v>137</v>
       </c>
@@ -5428,8 +5689,20 @@
         <f>SUM(DeMMO1!L180:L199)</f>
         <v>760</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="30" t="s">
+        <v>1425</v>
+      </c>
+      <c r="L13" s="30" t="s">
+        <v>1431</v>
+      </c>
+      <c r="O13" s="30" t="s">
+        <v>1425</v>
+      </c>
+      <c r="U13" s="30" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="34" t="s">
         <v>137</v>
       </c>
@@ -5463,8 +5736,17 @@
         <f>SUM(DeMMO1!L200:L220)</f>
         <v>323</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="O14" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="U14" s="30" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="34" t="s">
         <v>137</v>
       </c>
@@ -5498,8 +5780,17 @@
         <f>SUM(DeMMO1!L221:L238)</f>
         <v>828</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" s="30" t="s">
+        <v>1428</v>
+      </c>
+      <c r="L15" s="30">
+        <v>1</v>
+      </c>
+      <c r="U15" s="30" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="34" t="s">
         <v>137</v>
       </c>
@@ -5533,8 +5824,26 @@
         <f>SUM(DeMMO1!L239:L258)</f>
         <v>1440</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="30" t="s">
+        <v>1429</v>
+      </c>
+      <c r="M16" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="O16" s="30" t="s">
+        <v>1429</v>
+      </c>
+      <c r="S16" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="T16" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U16" s="30" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="34" t="s">
         <v>137</v>
       </c>
@@ -5568,8 +5877,26 @@
         <f>SUM(DeMMO1!L259:L279)</f>
         <v>839</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="L17" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="M17" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="O17" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="T17" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U17" s="30" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" s="34" t="s">
         <v>137</v>
       </c>
@@ -5603,8 +5930,26 @@
         <f>SUM(DeMMO1!L280:L300)</f>
         <v>283</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="L18" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="O18" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="S18" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="T18" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U18" s="30" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" s="34" t="s">
         <v>137</v>
       </c>
@@ -5638,8 +5983,29 @@
         <f>SUM(DeMMO1!L301:L309)</f>
         <v>2320</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="30" t="s">
+        <v>1429</v>
+      </c>
+      <c r="L19" s="30" t="s">
+        <v>1428</v>
+      </c>
+      <c r="M19" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="O19" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="S19" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="T19" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U19" s="30" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" s="34" t="s">
         <v>137</v>
       </c>
@@ -5673,8 +6039,20 @@
         <f>SUM(DeMMO1!L310:L331)</f>
         <v>1952</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="O20" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="S20" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U20" s="30" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="34" t="s">
         <v>137</v>
       </c>
@@ -5708,8 +6086,23 @@
         <f>SUM(DeMMO1!L332:L341)</f>
         <v>2660</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="L21" s="30" t="s">
+        <v>1430</v>
+      </c>
+      <c r="O21" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="T21" s="30" t="s">
+        <v>1426</v>
+      </c>
+      <c r="U21" s="30" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" s="36" t="s">
         <v>137</v>
       </c>
@@ -5744,7 +6137,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:21">
       <c r="A23" s="36" t="s">
         <v>137</v>
       </c>
@@ -5778,7 +6171,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:21">
       <c r="A24" s="36" t="s">
         <v>137</v>
       </c>
@@ -5812,7 +6205,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:21">
       <c r="A25" s="36" t="s">
         <v>137</v>
       </c>
@@ -5846,7 +6239,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:21">
       <c r="A26" s="36" t="s">
         <v>137</v>
       </c>
@@ -5880,7 +6273,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:21">
       <c r="A27" s="36" t="s">
         <v>137</v>
       </c>
@@ -5914,7 +6307,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:21">
       <c r="A28" s="36" t="s">
         <v>137</v>
       </c>
@@ -5948,7 +6341,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:21">
       <c r="A29" s="36" t="s">
         <v>137</v>
       </c>
@@ -5982,7 +6375,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:21">
       <c r="A30" s="36" t="s">
         <v>137</v>
       </c>
@@ -6016,7 +6409,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:21">
       <c r="A31" s="36" t="s">
         <v>137</v>
       </c>
@@ -6050,7 +6443,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:21">
       <c r="A32" s="36" t="s">
         <v>173</v>
       </c>
@@ -6085,7 +6478,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:21">
       <c r="A33" s="36" t="s">
         <v>173</v>
       </c>
@@ -6120,7 +6513,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:21">
       <c r="A34" s="36" t="s">
         <v>173</v>
       </c>
@@ -6153,7 +6546,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:21">
       <c r="A35" s="36" t="s">
         <v>173</v>
       </c>
@@ -6188,7 +6581,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:21">
       <c r="A36" s="36" t="s">
         <v>173</v>
       </c>
@@ -6223,7 +6616,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:21">
       <c r="A37" s="36" t="s">
         <v>173</v>
       </c>
@@ -6258,7 +6651,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:21">
       <c r="A38" s="36" t="s">
         <v>173</v>
       </c>
@@ -6293,7 +6686,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:21">
       <c r="A39" s="36" t="s">
         <v>173</v>
       </c>
@@ -6328,7 +6721,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="16" thickBot="1">
+    <row r="40" spans="1:21" ht="16" thickBot="1">
       <c r="A40" s="36" t="s">
         <v>173</v>
       </c>
@@ -6363,7 +6756,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="16" thickBot="1">
+    <row r="41" spans="1:21" ht="16" thickBot="1">
       <c r="A41" s="91" t="s">
         <v>173</v>
       </c>
@@ -6398,7 +6791,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:21">
       <c r="A42" s="34" t="s">
         <v>173</v>
       </c>
@@ -6433,7 +6826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="16" thickBot="1">
+    <row r="43" spans="1:21" ht="16" thickBot="1">
       <c r="A43" s="94" t="s">
         <v>173</v>
       </c>
@@ -6466,7 +6859,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="16" thickBot="1">
+    <row r="44" spans="1:21" ht="16" thickBot="1">
       <c r="A44" s="31" t="s">
         <v>173</v>
       </c>
@@ -6501,7 +6894,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="16" thickBot="1">
+    <row r="45" spans="1:21" ht="16" thickBot="1">
       <c r="A45" s="31" t="s">
         <v>173</v>
       </c>
@@ -6536,7 +6929,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="16" thickBot="1">
+    <row r="46" spans="1:21" ht="16" thickBot="1">
       <c r="A46" s="31" t="s">
         <v>173</v>
       </c>
@@ -6571,7 +6964,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="16" thickBot="1">
+    <row r="47" spans="1:21" ht="16" thickBot="1">
       <c r="A47" s="31" t="s">
         <v>173</v>
       </c>
@@ -6605,8 +6998,20 @@
         <f>SUM(DeMMO3!L218:L237)</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="16" thickBot="1">
+      <c r="K47" s="30" t="s">
+        <v>1429</v>
+      </c>
+      <c r="P47" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="Q47" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="U47" s="30" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="16" thickBot="1">
       <c r="A48" s="31" t="s">
         <v>173</v>
       </c>
@@ -6641,7 +7046,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="16" thickBot="1">
+    <row r="49" spans="1:21" ht="16" thickBot="1">
       <c r="A49" s="91" t="s">
         <v>175</v>
       </c>
@@ -6674,8 +7079,17 @@
         <f>SUM(DeMMO3!L258:L277)</f>
         <v>132</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="16" thickBot="1">
+      <c r="K49" s="30" t="s">
+        <v>1425</v>
+      </c>
+      <c r="L49" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="U49" s="30" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="16" thickBot="1">
       <c r="A50" s="91" t="s">
         <v>175</v>
       </c>
@@ -6709,7 +7123,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="16" thickBot="1">
+    <row r="51" spans="1:21" ht="16" thickBot="1">
       <c r="A51" s="91" t="s">
         <v>175</v>
       </c>
@@ -6742,8 +7156,20 @@
         <f>SUM(DeMMO3!L300:L319)</f>
         <v>98</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="16" thickBot="1">
+      <c r="K51" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="L51" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="P51" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="U51" s="30" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="16" thickBot="1">
       <c r="A52" s="91" t="s">
         <v>175</v>
       </c>
@@ -6777,7 +7203,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="16" thickBot="1">
+    <row r="53" spans="1:21" ht="16" thickBot="1">
       <c r="A53" s="91" t="s">
         <v>175</v>
       </c>
@@ -6811,7 +7237,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="16" thickBot="1">
+    <row r="54" spans="1:21" ht="16" thickBot="1">
       <c r="A54" s="91" t="s">
         <v>175</v>
       </c>
@@ -6845,7 +7271,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="16" thickBot="1">
+    <row r="55" spans="1:21" ht="16" thickBot="1">
       <c r="A55" s="91" t="s">
         <v>175</v>
       </c>
@@ -6877,7 +7303,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="16" thickBot="1">
+    <row r="56" spans="1:21" ht="16" thickBot="1">
       <c r="A56" s="91" t="s">
         <v>175</v>
       </c>
@@ -6911,7 +7337,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="16" thickBot="1">
+    <row r="57" spans="1:21" ht="16" thickBot="1">
       <c r="A57" s="91" t="s">
         <v>175</v>
       </c>
@@ -6946,7 +7372,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="16" thickBot="1">
+    <row r="58" spans="1:21" ht="16" thickBot="1">
       <c r="A58" s="91" t="s">
         <v>175</v>
       </c>
@@ -6979,7 +7405,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="16" thickBot="1">
+    <row r="59" spans="1:21" ht="16" thickBot="1">
       <c r="A59" s="91" t="s">
         <v>175</v>
       </c>
@@ -7014,7 +7440,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="16" thickBot="1">
+    <row r="60" spans="1:21" ht="16" thickBot="1">
       <c r="A60" s="91" t="s">
         <v>175</v>
       </c>
@@ -7049,7 +7475,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="16" thickBot="1">
+    <row r="61" spans="1:21" ht="16" thickBot="1">
       <c r="A61" s="97" t="s">
         <v>175</v>
       </c>
@@ -7084,7 +7510,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="16" thickBot="1">
+    <row r="62" spans="1:21" ht="16" thickBot="1">
       <c r="A62" s="91" t="s">
         <v>175</v>
       </c>
@@ -7119,7 +7545,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:21">
       <c r="A63" s="34" t="s">
         <v>175</v>
       </c>
@@ -7154,7 +7580,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:21">
       <c r="A64" s="34" t="s">
         <v>175</v>
       </c>
@@ -7426,6 +7852,7 @@
         <f>SUM(DeMMO6!L62:L71)</f>
         <v>352</v>
       </c>
+      <c r="L71" s="100"/>
       <c r="M71" s="100"/>
     </row>
     <row r="72" spans="1:13" ht="16" thickBot="1">
@@ -7461,6 +7888,7 @@
         <f>SUM(DeMMO6!L72:L91)</f>
         <v>1</v>
       </c>
+      <c r="L72" s="100"/>
       <c r="M72" s="100"/>
     </row>
     <row r="73" spans="1:13" ht="16" thickBot="1">
@@ -7496,6 +7924,7 @@
         <f>SUM(DeMMO6!L92:L111)</f>
         <v>678</v>
       </c>
+      <c r="L73" s="100"/>
       <c r="M73" s="100"/>
     </row>
     <row r="74" spans="1:13" ht="16" thickBot="1">
@@ -7531,6 +7960,7 @@
         <f>SUM(DeMMO6!L112:L121)</f>
         <v>897</v>
       </c>
+      <c r="L74" s="100"/>
       <c r="M74" s="100"/>
     </row>
     <row r="75" spans="1:13" ht="16" thickBot="1">
@@ -7564,6 +7994,7 @@
       <c r="J75" s="30" t="s">
         <v>179</v>
       </c>
+      <c r="L75" s="100"/>
       <c r="M75" s="100"/>
     </row>
     <row r="76" spans="1:13" ht="16" thickBot="1">
@@ -7599,6 +8030,7 @@
         <f>SUM(DeMMO6!L122:L131)</f>
         <v>594</v>
       </c>
+      <c r="L76" s="100"/>
       <c r="M76" s="100"/>
     </row>
     <row r="77" spans="1:13" ht="16" thickBot="1">
@@ -7634,6 +8066,7 @@
         <f>SUM(DeMMO6!L132:L151)</f>
         <v>361</v>
       </c>
+      <c r="L77" s="100"/>
       <c r="M77" s="100"/>
     </row>
     <row r="78" spans="1:13" ht="16" thickBot="1">
@@ -7667,6 +8100,7 @@
       <c r="J78" s="30" t="s">
         <v>179</v>
       </c>
+      <c r="L78" s="100"/>
       <c r="M78" s="100"/>
     </row>
     <row r="79" spans="1:13" ht="16" thickBot="1">
@@ -7702,6 +8136,7 @@
         <f>SUM(DeMMO6!L152:L161)</f>
         <v>406</v>
       </c>
+      <c r="L79" s="100"/>
       <c r="M79" s="100"/>
     </row>
     <row r="80" spans="1:13" ht="16" thickBot="1">
@@ -7737,6 +8172,7 @@
         <f>SUM(DeMMO6!L162:L181)</f>
         <v>288</v>
       </c>
+      <c r="L80" s="100"/>
       <c r="M80" s="100"/>
     </row>
     <row r="81" spans="1:10" ht="16" thickBot="1">
@@ -15558,7 +15994,7 @@
   <sheetViews>
     <sheetView zoomScale="118" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -34813,9 +35249,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596C5F9B-0BCC-432C-9C10-F3730A593712}">
   <dimension ref="A1:S552"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A336" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M355" sqref="M355"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -57029,8 +57465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F7FECC-F9BB-4ECA-A2C2-80FEA331CA5F}">
   <dimension ref="A1:L241"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M221" sqref="M221"/>
     </sheetView>
   </sheetViews>

</xml_diff>